<commit_message>
Data updated until 09.09.2023
</commit_message>
<xml_diff>
--- a/Data Files/bitcoin/xlsx Files/bitcoin.com_news_Test_Data_Sentiments.xlsx
+++ b/Data Files/bitcoin/xlsx Files/bitcoin.com_news_Test_Data_Sentiments.xlsx
@@ -380,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1291"/>
+  <dimension ref="A1:D1314"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -18460,6 +18460,328 @@
         <v>0</v>
       </c>
     </row>
+    <row r="1292" spans="1:4">
+      <c r="A1292" s="2">
+        <v>45156</v>
+      </c>
+      <c r="B1292">
+        <v>4</v>
+      </c>
+      <c r="C1292">
+        <v>0</v>
+      </c>
+      <c r="D1292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:4">
+      <c r="A1293" s="2">
+        <v>45157</v>
+      </c>
+      <c r="B1293">
+        <v>1</v>
+      </c>
+      <c r="C1293">
+        <v>0</v>
+      </c>
+      <c r="D1293">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:4">
+      <c r="A1294" s="2">
+        <v>45158</v>
+      </c>
+      <c r="B1294">
+        <v>2</v>
+      </c>
+      <c r="C1294">
+        <v>0</v>
+      </c>
+      <c r="D1294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:4">
+      <c r="A1295" s="2">
+        <v>45159</v>
+      </c>
+      <c r="B1295">
+        <v>4</v>
+      </c>
+      <c r="C1295">
+        <v>0</v>
+      </c>
+      <c r="D1295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:4">
+      <c r="A1296" s="2">
+        <v>45160</v>
+      </c>
+      <c r="B1296">
+        <v>2</v>
+      </c>
+      <c r="C1296">
+        <v>0</v>
+      </c>
+      <c r="D1296">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:4">
+      <c r="A1297" s="2">
+        <v>45161</v>
+      </c>
+      <c r="B1297">
+        <v>3</v>
+      </c>
+      <c r="C1297">
+        <v>0</v>
+      </c>
+      <c r="D1297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:4">
+      <c r="A1298" s="2">
+        <v>45162</v>
+      </c>
+      <c r="B1298">
+        <v>3</v>
+      </c>
+      <c r="C1298">
+        <v>0</v>
+      </c>
+      <c r="D1298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:4">
+      <c r="A1299" s="2">
+        <v>45163</v>
+      </c>
+      <c r="B1299">
+        <v>1</v>
+      </c>
+      <c r="C1299">
+        <v>0</v>
+      </c>
+      <c r="D1299">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:4">
+      <c r="A1300" s="2">
+        <v>45164</v>
+      </c>
+      <c r="B1300">
+        <v>1</v>
+      </c>
+      <c r="C1300">
+        <v>0</v>
+      </c>
+      <c r="D1300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:4">
+      <c r="A1301" s="2">
+        <v>45165</v>
+      </c>
+      <c r="B1301">
+        <v>2</v>
+      </c>
+      <c r="C1301">
+        <v>0</v>
+      </c>
+      <c r="D1301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:4">
+      <c r="A1302" s="2">
+        <v>45166</v>
+      </c>
+      <c r="B1302">
+        <v>2</v>
+      </c>
+      <c r="C1302">
+        <v>0</v>
+      </c>
+      <c r="D1302">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:4">
+      <c r="A1303" s="2">
+        <v>45167</v>
+      </c>
+      <c r="B1303">
+        <v>5</v>
+      </c>
+      <c r="C1303">
+        <v>0</v>
+      </c>
+      <c r="D1303">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:4">
+      <c r="A1304" s="2">
+        <v>45168</v>
+      </c>
+      <c r="B1304">
+        <v>4</v>
+      </c>
+      <c r="C1304">
+        <v>0</v>
+      </c>
+      <c r="D1304">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:4">
+      <c r="A1305" s="2">
+        <v>45169</v>
+      </c>
+      <c r="B1305">
+        <v>4</v>
+      </c>
+      <c r="C1305">
+        <v>0</v>
+      </c>
+      <c r="D1305">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:4">
+      <c r="A1306" s="2">
+        <v>45170</v>
+      </c>
+      <c r="B1306">
+        <v>3</v>
+      </c>
+      <c r="C1306">
+        <v>0</v>
+      </c>
+      <c r="D1306">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:4">
+      <c r="A1307" s="2">
+        <v>45171</v>
+      </c>
+      <c r="B1307">
+        <v>3</v>
+      </c>
+      <c r="C1307">
+        <v>0</v>
+      </c>
+      <c r="D1307">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:4">
+      <c r="A1308" s="2">
+        <v>45172</v>
+      </c>
+      <c r="B1308">
+        <v>3</v>
+      </c>
+      <c r="C1308">
+        <v>0</v>
+      </c>
+      <c r="D1308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:4">
+      <c r="A1309" s="2">
+        <v>45173</v>
+      </c>
+      <c r="B1309">
+        <v>2</v>
+      </c>
+      <c r="C1309">
+        <v>0</v>
+      </c>
+      <c r="D1309">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:4">
+      <c r="A1310" s="2">
+        <v>45174</v>
+      </c>
+      <c r="B1310">
+        <v>2</v>
+      </c>
+      <c r="C1310">
+        <v>0</v>
+      </c>
+      <c r="D1310">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:4">
+      <c r="A1311" s="2">
+        <v>45175</v>
+      </c>
+      <c r="B1311">
+        <v>9</v>
+      </c>
+      <c r="C1311">
+        <v>0</v>
+      </c>
+      <c r="D1311">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:4">
+      <c r="A1312" s="2">
+        <v>45176</v>
+      </c>
+      <c r="B1312">
+        <v>4</v>
+      </c>
+      <c r="C1312">
+        <v>0</v>
+      </c>
+      <c r="D1312">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:4">
+      <c r="A1313" s="2">
+        <v>45177</v>
+      </c>
+      <c r="B1313">
+        <v>2</v>
+      </c>
+      <c r="C1313">
+        <v>0</v>
+      </c>
+      <c r="D1313">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:4">
+      <c r="A1314" s="2">
+        <v>45178</v>
+      </c>
+      <c r="B1314">
+        <v>3</v>
+      </c>
+      <c r="C1314">
+        <v>0</v>
+      </c>
+      <c r="D1314">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed news part's errors
</commit_message>
<xml_diff>
--- a/Data Files/bitcoin/xlsx Files/bitcoin.com_news_Test_Data_Sentiments.xlsx
+++ b/Data Files/bitcoin/xlsx Files/bitcoin.com_news_Test_Data_Sentiments.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1326"/>
+  <dimension ref="A1:D1465"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19005,6 +19005,1952 @@
         <v>0</v>
       </c>
     </row>
+    <row r="1327">
+      <c r="A1327" s="2" t="n">
+        <v>45208</v>
+      </c>
+      <c r="B1327" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1327" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1327" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" s="2" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B1328" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1328" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1328" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" s="2" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B1329" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1329" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1329" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" s="2" t="n">
+        <v>45211</v>
+      </c>
+      <c r="B1330" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1330" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1330" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" s="2" t="n">
+        <v>45212</v>
+      </c>
+      <c r="B1331" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1331" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1331" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" s="2" t="n">
+        <v>45213</v>
+      </c>
+      <c r="B1332" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1332" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1332" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" s="2" t="n">
+        <v>45214</v>
+      </c>
+      <c r="B1333" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1333" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1333" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" s="2" t="n">
+        <v>45215</v>
+      </c>
+      <c r="B1334" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1334" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1334" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" s="2" t="n">
+        <v>45216</v>
+      </c>
+      <c r="B1335" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1335" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1335" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" s="2" t="n">
+        <v>45217</v>
+      </c>
+      <c r="B1336" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1336" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1336" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" s="2" t="n">
+        <v>45218</v>
+      </c>
+      <c r="B1337" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1337" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1337" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" s="2" t="n">
+        <v>45219</v>
+      </c>
+      <c r="B1338" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1338" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1338" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" s="2" t="n">
+        <v>45220</v>
+      </c>
+      <c r="B1339" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1339" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1339" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" s="2" t="n">
+        <v>45221</v>
+      </c>
+      <c r="B1340" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1340" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1340" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" s="2" t="n">
+        <v>45222</v>
+      </c>
+      <c r="B1341" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1341" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1341" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" s="2" t="n">
+        <v>45223</v>
+      </c>
+      <c r="B1342" t="n">
+        <v>6</v>
+      </c>
+      <c r="C1342" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1342" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" s="2" t="n">
+        <v>45224</v>
+      </c>
+      <c r="B1343" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1343" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1343" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" s="2" t="n">
+        <v>45225</v>
+      </c>
+      <c r="B1344" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1344" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1344" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" s="2" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B1345" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1345" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1345" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" s="2" t="n">
+        <v>45227</v>
+      </c>
+      <c r="B1346" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1346" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1346" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" s="2" t="n">
+        <v>45228</v>
+      </c>
+      <c r="B1347" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1347" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1347" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" s="2" t="n">
+        <v>45229</v>
+      </c>
+      <c r="B1348" t="n">
+        <v>6</v>
+      </c>
+      <c r="C1348" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1348" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" s="2" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B1349" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1349" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1349" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" s="2" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B1350" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1350" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1350" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" s="2" t="n">
+        <v>45232</v>
+      </c>
+      <c r="B1351" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1351" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1351" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" s="2" t="n">
+        <v>45233</v>
+      </c>
+      <c r="B1352" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1352" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1352" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" s="2" t="n">
+        <v>45234</v>
+      </c>
+      <c r="B1353" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1353" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1353" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" s="2" t="n">
+        <v>45235</v>
+      </c>
+      <c r="B1354" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1354" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1354" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" s="2" t="n">
+        <v>45236</v>
+      </c>
+      <c r="B1355" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1355" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1355" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" s="2" t="n">
+        <v>45237</v>
+      </c>
+      <c r="B1356" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1356" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1356" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" s="2" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B1357" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1357" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1357" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="B1358" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1358" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1358" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="B1359" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1359" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1359" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" s="2" t="n">
+        <v>45241</v>
+      </c>
+      <c r="B1360" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1360" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1360" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" s="2" t="n">
+        <v>45242</v>
+      </c>
+      <c r="B1361" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1361" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1361" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" s="2" t="n">
+        <v>45243</v>
+      </c>
+      <c r="B1362" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1362" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1362" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" s="2" t="n">
+        <v>45244</v>
+      </c>
+      <c r="B1363" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1363" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1363" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" s="2" t="n">
+        <v>45245</v>
+      </c>
+      <c r="B1364" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1364" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1364" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" s="2" t="n">
+        <v>45246</v>
+      </c>
+      <c r="B1365" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1365" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1365" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" s="2" t="n">
+        <v>45247</v>
+      </c>
+      <c r="B1366" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1366" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1366" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" s="2" t="n">
+        <v>45248</v>
+      </c>
+      <c r="B1367" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1367" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1367" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" s="2" t="n">
+        <v>45249</v>
+      </c>
+      <c r="B1368" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1368" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1368" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" s="2" t="n">
+        <v>45250</v>
+      </c>
+      <c r="B1369" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1369" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1369" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" s="2" t="n">
+        <v>45251</v>
+      </c>
+      <c r="B1370" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1370" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1370" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" s="2" t="n">
+        <v>45252</v>
+      </c>
+      <c r="B1371" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1371" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1371" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" s="2" t="n">
+        <v>45253</v>
+      </c>
+      <c r="B1372" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1372" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1372" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" s="2" t="n">
+        <v>45254</v>
+      </c>
+      <c r="B1373" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1373" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1373" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" s="2" t="n">
+        <v>45255</v>
+      </c>
+      <c r="B1374" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1374" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1374" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" s="2" t="n">
+        <v>45256</v>
+      </c>
+      <c r="B1375" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1375" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1375" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" s="2" t="n">
+        <v>45257</v>
+      </c>
+      <c r="B1376" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1376" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1376" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" s="2" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B1377" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1377" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1377" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" s="2" t="n">
+        <v>45259</v>
+      </c>
+      <c r="B1378" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1378" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1378" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" s="2" t="n">
+        <v>45260</v>
+      </c>
+      <c r="B1379" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1379" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1379" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" s="2" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B1380" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1380" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1380" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" s="2" t="n">
+        <v>45262</v>
+      </c>
+      <c r="B1381" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1381" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1381" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" s="2" t="n">
+        <v>45263</v>
+      </c>
+      <c r="B1382" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1382" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1382" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" s="2" t="n">
+        <v>45264</v>
+      </c>
+      <c r="B1383" t="n">
+        <v>7</v>
+      </c>
+      <c r="C1383" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1383" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" s="2" t="n">
+        <v>45265</v>
+      </c>
+      <c r="B1384" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1384" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1384" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" s="2" t="n">
+        <v>45266</v>
+      </c>
+      <c r="B1385" t="n">
+        <v>7</v>
+      </c>
+      <c r="C1385" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1385" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" s="2" t="n">
+        <v>45267</v>
+      </c>
+      <c r="B1386" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1386" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1386" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" s="2" t="n">
+        <v>45268</v>
+      </c>
+      <c r="B1387" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1387" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1387" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" s="2" t="n">
+        <v>45269</v>
+      </c>
+      <c r="B1388" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1388" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1388" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" s="2" t="n">
+        <v>45270</v>
+      </c>
+      <c r="B1389" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1389" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1389" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" s="2" t="n">
+        <v>45271</v>
+      </c>
+      <c r="B1390" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1390" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1390" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" s="2" t="n">
+        <v>45272</v>
+      </c>
+      <c r="B1391" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1391" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1391" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" s="2" t="n">
+        <v>45273</v>
+      </c>
+      <c r="B1392" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1392" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1392" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" s="2" t="n">
+        <v>45274</v>
+      </c>
+      <c r="B1393" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1393" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1393" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" s="2" t="n">
+        <v>45275</v>
+      </c>
+      <c r="B1394" t="n">
+        <v>6</v>
+      </c>
+      <c r="C1394" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1394" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" s="2" t="n">
+        <v>45276</v>
+      </c>
+      <c r="B1395" t="n">
+        <v>6</v>
+      </c>
+      <c r="C1395" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1395" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" s="2" t="n">
+        <v>45277</v>
+      </c>
+      <c r="B1396" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1396" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1396" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" s="2" t="n">
+        <v>45278</v>
+      </c>
+      <c r="B1397" t="n">
+        <v>9</v>
+      </c>
+      <c r="C1397" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1397" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" s="2" t="n">
+        <v>45279</v>
+      </c>
+      <c r="B1398" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1398" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1398" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" s="2" t="n">
+        <v>45280</v>
+      </c>
+      <c r="B1399" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1399" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1399" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" s="2" t="n">
+        <v>45281</v>
+      </c>
+      <c r="B1400" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1400" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1400" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" s="2" t="n">
+        <v>45282</v>
+      </c>
+      <c r="B1401" t="n">
+        <v>6</v>
+      </c>
+      <c r="C1401" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1401" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" s="2" t="n">
+        <v>45283</v>
+      </c>
+      <c r="B1402" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1402" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1402" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" s="2" t="n">
+        <v>45284</v>
+      </c>
+      <c r="B1403" t="n">
+        <v>7</v>
+      </c>
+      <c r="C1403" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1403" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" s="2" t="n">
+        <v>45285</v>
+      </c>
+      <c r="B1404" t="n">
+        <v>6</v>
+      </c>
+      <c r="C1404" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1404" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" s="2" t="n">
+        <v>45286</v>
+      </c>
+      <c r="B1405" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1405" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1405" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" s="2" t="n">
+        <v>45287</v>
+      </c>
+      <c r="B1406" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1406" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1406" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" s="2" t="n">
+        <v>45288</v>
+      </c>
+      <c r="B1407" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1407" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1407" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" s="2" t="n">
+        <v>45289</v>
+      </c>
+      <c r="B1408" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1408" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1408" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" s="2" t="n">
+        <v>45290</v>
+      </c>
+      <c r="B1409" t="n">
+        <v>7</v>
+      </c>
+      <c r="C1409" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1409" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" s="2" t="n">
+        <v>45291</v>
+      </c>
+      <c r="B1410" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1410" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1410" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" s="2" t="n">
+        <v>45292</v>
+      </c>
+      <c r="B1411" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1411" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1411" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" s="2" t="n">
+        <v>45293</v>
+      </c>
+      <c r="B1412" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1412" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1412" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" s="2" t="n">
+        <v>45294</v>
+      </c>
+      <c r="B1413" t="n">
+        <v>9</v>
+      </c>
+      <c r="C1413" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1413" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" s="2" t="n">
+        <v>45295</v>
+      </c>
+      <c r="B1414" t="n">
+        <v>7</v>
+      </c>
+      <c r="C1414" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1414" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" s="2" t="n">
+        <v>45296</v>
+      </c>
+      <c r="B1415" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1415" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1415" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" s="2" t="n">
+        <v>45297</v>
+      </c>
+      <c r="B1416" t="n">
+        <v>7</v>
+      </c>
+      <c r="C1416" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1416" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" s="2" t="n">
+        <v>45298</v>
+      </c>
+      <c r="B1417" t="n">
+        <v>6</v>
+      </c>
+      <c r="C1417" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1417" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" s="2" t="n">
+        <v>45299</v>
+      </c>
+      <c r="B1418" t="n">
+        <v>9</v>
+      </c>
+      <c r="C1418" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1418" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" s="2" t="n">
+        <v>45300</v>
+      </c>
+      <c r="B1419" t="n">
+        <v>10</v>
+      </c>
+      <c r="C1419" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1419" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" s="2" t="n">
+        <v>45301</v>
+      </c>
+      <c r="B1420" t="n">
+        <v>12</v>
+      </c>
+      <c r="C1420" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1420" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" s="2" t="n">
+        <v>45302</v>
+      </c>
+      <c r="B1421" t="n">
+        <v>9</v>
+      </c>
+      <c r="C1421" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1421" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" s="2" t="n">
+        <v>45303</v>
+      </c>
+      <c r="B1422" t="n">
+        <v>11</v>
+      </c>
+      <c r="C1422" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1422" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" s="2" t="n">
+        <v>45304</v>
+      </c>
+      <c r="B1423" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1423" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1423" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" s="2" t="n">
+        <v>45305</v>
+      </c>
+      <c r="B1424" t="n">
+        <v>9</v>
+      </c>
+      <c r="C1424" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1424" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" s="2" t="n">
+        <v>45306</v>
+      </c>
+      <c r="B1425" t="n">
+        <v>6</v>
+      </c>
+      <c r="C1425" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1425" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" s="2" t="n">
+        <v>45307</v>
+      </c>
+      <c r="B1426" t="n">
+        <v>6</v>
+      </c>
+      <c r="C1426" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1426" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" s="2" t="n">
+        <v>45308</v>
+      </c>
+      <c r="B1427" t="n">
+        <v>7</v>
+      </c>
+      <c r="C1427" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1427" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" s="2" t="n">
+        <v>45309</v>
+      </c>
+      <c r="B1428" t="n">
+        <v>7</v>
+      </c>
+      <c r="C1428" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1428" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" s="2" t="n">
+        <v>45310</v>
+      </c>
+      <c r="B1429" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1429" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1429" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" s="2" t="n">
+        <v>45311</v>
+      </c>
+      <c r="B1430" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1430" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1430" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" s="2" t="n">
+        <v>45312</v>
+      </c>
+      <c r="B1431" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1431" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1431" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" s="2" t="n">
+        <v>45313</v>
+      </c>
+      <c r="B1432" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1432" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1432" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" s="2" t="n">
+        <v>45314</v>
+      </c>
+      <c r="B1433" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1433" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1433" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="B1434" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1434" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1434" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" s="2" t="n">
+        <v>45316</v>
+      </c>
+      <c r="B1435" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1435" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1435" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" s="2" t="n">
+        <v>45317</v>
+      </c>
+      <c r="B1436" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1436" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1436" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" s="2" t="n">
+        <v>45318</v>
+      </c>
+      <c r="B1437" t="n">
+        <v>6</v>
+      </c>
+      <c r="C1437" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1437" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" s="2" t="n">
+        <v>45319</v>
+      </c>
+      <c r="B1438" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1438" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1438" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" s="2" t="n">
+        <v>45320</v>
+      </c>
+      <c r="B1439" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1439" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1439" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" s="2" t="n">
+        <v>45321</v>
+      </c>
+      <c r="B1440" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1440" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1440" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" s="2" t="n">
+        <v>45322</v>
+      </c>
+      <c r="B1441" t="n">
+        <v>7</v>
+      </c>
+      <c r="C1441" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1441" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" s="2" t="n">
+        <v>45323</v>
+      </c>
+      <c r="B1442" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1442" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1442" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" s="2" t="n">
+        <v>45324</v>
+      </c>
+      <c r="B1443" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1443" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1443" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" s="2" t="n">
+        <v>45325</v>
+      </c>
+      <c r="B1444" t="n">
+        <v>6</v>
+      </c>
+      <c r="C1444" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1444" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" s="2" t="n">
+        <v>45326</v>
+      </c>
+      <c r="B1445" t="n">
+        <v>6</v>
+      </c>
+      <c r="C1445" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1445" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" s="2" t="n">
+        <v>45327</v>
+      </c>
+      <c r="B1446" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1446" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1446" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" s="2" t="n">
+        <v>45328</v>
+      </c>
+      <c r="B1447" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1447" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1447" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" s="2" t="n">
+        <v>45329</v>
+      </c>
+      <c r="B1448" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1448" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1448" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" s="2" t="n">
+        <v>45330</v>
+      </c>
+      <c r="B1449" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1449" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1449" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" s="2" t="n">
+        <v>45331</v>
+      </c>
+      <c r="B1450" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1450" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1450" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" s="2" t="n">
+        <v>45332</v>
+      </c>
+      <c r="B1451" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1451" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1451" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" s="2" t="n">
+        <v>45333</v>
+      </c>
+      <c r="B1452" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1452" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1452" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" s="2" t="n">
+        <v>45334</v>
+      </c>
+      <c r="B1453" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1453" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1453" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" s="2" t="n">
+        <v>45335</v>
+      </c>
+      <c r="B1454" t="n">
+        <v>7</v>
+      </c>
+      <c r="C1454" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1454" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" s="2" t="n">
+        <v>45336</v>
+      </c>
+      <c r="B1455" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1455" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1455" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" s="2" t="n">
+        <v>45337</v>
+      </c>
+      <c r="B1456" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1456" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1456" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" s="2" t="n">
+        <v>45338</v>
+      </c>
+      <c r="B1457" t="n">
+        <v>6</v>
+      </c>
+      <c r="C1457" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1457" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" s="2" t="n">
+        <v>45339</v>
+      </c>
+      <c r="B1458" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1458" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1458" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" s="2" t="n">
+        <v>45340</v>
+      </c>
+      <c r="B1459" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1459" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1459" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" s="2" t="n">
+        <v>45341</v>
+      </c>
+      <c r="B1460" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1460" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1460" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" s="2" t="n">
+        <v>45342</v>
+      </c>
+      <c r="B1461" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1461" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1461" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" s="2" t="n">
+        <v>45343</v>
+      </c>
+      <c r="B1462" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1462" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1462" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" s="2" t="n">
+        <v>45344</v>
+      </c>
+      <c r="B1463" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1463" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1463" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" s="2" t="n">
+        <v>45345</v>
+      </c>
+      <c r="B1464" t="n">
+        <v>6</v>
+      </c>
+      <c r="C1464" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1464" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" s="2" t="n">
+        <v>45346</v>
+      </c>
+      <c r="B1465" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1465" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1465" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>